<commit_message>
results, metamodel, and example modeled updated
</commit_message>
<xml_diff>
--- a/experimental-validation/experiment-1-mining-participants/Results.xlsx
+++ b/experimental-validation/experiment-1-mining-participants/Results.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DellPhoto\Documents\Github\IoT-Mining-DSL\experimental-validation\experiment-1-mining-participants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5971E4DF-E82A-4C8D-993A-F40045AA3E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F6C3BD-D734-4B26-A3B8-7E7C92612F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{316D7274-BD52-4D7F-AE2D-2EF32EDE85AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{316D7274-BD52-4D7F-AE2D-2EF32EDE85AF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Q0" sheetId="3" r:id="rId1"/>
-    <sheet name="Q1" sheetId="4" r:id="rId2"/>
-    <sheet name="Q2" sheetId="5" r:id="rId3"/>
-    <sheet name="Modeling errors" sheetId="2" r:id="rId4"/>
+    <sheet name="Encuesta 1" sheetId="3" r:id="rId1"/>
+    <sheet name="Encuesta 2" sheetId="4" r:id="rId2"/>
+    <sheet name="Encuesta 3" sheetId="5" r:id="rId3"/>
+    <sheet name="Errores en los modelos" sheetId="2" r:id="rId4"/>
+    <sheet name="Graphs" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,9 +39,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="91">
+  <si>
+    <t>Regiones</t>
+  </si>
+  <si>
+    <t>Puntos de control</t>
+  </si>
+  <si>
+    <t>Sensores</t>
+  </si>
+  <si>
+    <t>Actuadores</t>
+  </si>
+  <si>
+    <t>Condicion</t>
+  </si>
+  <si>
+    <t>Adaptacion</t>
+  </si>
+  <si>
+    <t>Regla 1</t>
+  </si>
+  <si>
+    <t>Regla 2</t>
+  </si>
+  <si>
+    <t>Regla 3</t>
+  </si>
+  <si>
+    <t>Errores</t>
+  </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Teimpo E1 (min)</t>
+  </si>
+  <si>
+    <t>Tiempo E2 (min)</t>
   </si>
   <si>
     <t>#</t>
@@ -259,27 +296,6 @@
     <t>Participante</t>
   </si>
   <si>
-    <t>Muy alto</t>
-  </si>
-  <si>
-    <t>Errors</t>
-  </si>
-  <si>
-    <t>Rule 1</t>
-  </si>
-  <si>
-    <t>Rule 2</t>
-  </si>
-  <si>
-    <t>Rule 3</t>
-  </si>
-  <si>
-    <t>Condition</t>
-  </si>
-  <si>
-    <t>Adaptation</t>
-  </si>
-  <si>
     <t>Regions</t>
   </si>
   <si>
@@ -292,12 +308,34 @@
     <t>Actuators</t>
   </si>
   <si>
-    <t>Time E1
-(min)</t>
-  </si>
-  <si>
-    <t>Time E2
-(min)</t>
+    <t>Rule-conditions</t>
+  </si>
+  <si>
+    <t>Rule-actions</t>
+  </si>
+  <si>
+    <t>Mine structure</t>
+  </si>
+  <si>
+    <t>Control points, sensors and actuators</t>
+  </si>
+  <si>
+    <t>Adaptation rules</t>
+  </si>
+  <si>
+    <t>Very easy</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Correctly modeled</t>
+  </si>
+  <si>
+    <t>Incorrectly modeled</t>
   </si>
 </sst>
 </file>
@@ -411,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -455,6 +493,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -489,6 +530,2240 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Mine structure</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.2388888888888889"/>
+                  <c:y val="-4.6296296296296294E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-95A1-4543-8A88-D93B0417F110}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.3527777777777778"/>
+                  <c:y val="-9.2592592592592587E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-95A1-4543-8A88-D93B0417F110}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.16944444444444443"/>
+                  <c:y val="4.6296296296296294E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-95A1-4543-8A88-D93B0417F110}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$B$20:$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Very easy</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Easy</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Medium</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Very easy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Easy</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Easy</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Medium</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$C$20:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-95A1-4543-8A88-D93B0417F110}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Control points, sensors and actuators</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.19999999999999996"/>
+                  <c:y val="-9.2592592592592587E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-95A1-4543-8A88-D93B0417F110}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.48055555555555557"/>
+                  <c:y val="4.6296296296296294E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-95A1-4543-8A88-D93B0417F110}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$B$20:$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Very easy</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Easy</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Medium</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Very easy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Easy</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Easy</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Medium</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$D$20:$D$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="3" formatCode="0%">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0%">
+                  <c:v>0.87</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-95A1-4543-8A88-D93B0417F110}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Adaptation rules</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.39444444444444443"/>
+                  <c:y val="-2.1218890680033321E-17"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-95A1-4543-8A88-D93B0417F110}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.28611111111111115"/>
+                  <c:y val="4.6296296296296294E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-95A1-4543-8A88-D93B0417F110}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$B$20:$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Very easy</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Easy</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Medium</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Very easy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Easy</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Easy</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Medium</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$E$20:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="5" formatCode="0%">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0%">
+                  <c:v>0.375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-95A1-4543-8A88-D93B0417F110}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="706917024"/>
+        <c:axId val="706918688"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="706917024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="706918688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="706918688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="706917024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graphs!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Correctly modeled</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$B$3:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Regions</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Control points</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sensors</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Actuators</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Rule-conditions</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Rule-actions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8571428571428571</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-44D9-494C-BC04-A442847E2117}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graphs!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Incorrectly modeled</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Graphs!$B$3:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Regions</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Control points</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sensors</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Actuators</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Rule-conditions</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Rule-actions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graphs!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.5714285714285712E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1428571428571425E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14285714285714285</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-44D9-494C-BC04-A442847E2117}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="567641551"/>
+        <c:axId val="567646959"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="567641551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="567646959"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="567646959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="567641551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55C28ACF-3D88-7C17-1148-2C3B5BB5415B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85786710-467D-B9E0-6234-6722A7B7F9D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -790,8 +3065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAF96150-DA40-4EC8-A2A1-875E180D2397}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,31 +3084,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="5" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -841,28 +3116,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -870,28 +3145,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -899,28 +3174,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -928,28 +3203,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -957,28 +3232,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -986,28 +3261,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" t="s">
-        <v>22</v>
+        <v>31</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1015,28 +3290,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1044,28 +3319,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" t="s">
         <v>34</v>
       </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" t="s">
-        <v>22</v>
-      </c>
       <c r="I9" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1097,31 +3372,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1129,16 +3404,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -1146,19 +3421,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -1166,16 +3441,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1183,19 +3458,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -1203,19 +3478,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -1223,22 +3498,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
@@ -1246,22 +3521,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1269,16 +3544,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1343,7 +3618,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1358,22 +3633,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1381,19 +3656,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1401,19 +3676,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1421,19 +3696,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
@@ -1441,19 +3716,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1461,19 +3736,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="144" x14ac:dyDescent="0.3">
@@ -1481,19 +3756,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1501,19 +3776,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1521,19 +3796,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1547,7 +3822,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1567,83 +3842,83 @@
     <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="21"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="M2" s="23"/>
+      <c r="F2" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="24"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="1" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1751,7 +4026,7 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1976,7 +4251,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3">
         <f>AVERAGE(B4:B10)</f>
@@ -2004,7 +4279,7 @@
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
@@ -2077,4 +4352,175 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A455FC-9176-4410-9CB7-E1069F926B92}">
+  <dimension ref="B2:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C2" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="17">
+        <v>0.96</v>
+      </c>
+      <c r="D3" s="17">
+        <f>2/56</f>
+        <v>3.5714285714285712E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="17">
+        <v>1</v>
+      </c>
+      <c r="D4" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="17">
+        <f>39/42</f>
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="D5" s="17">
+        <f>3/42</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="17">
+        <f>24/28</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="D6" s="17">
+        <f>4/28</f>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0.88</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="17">
+        <v>1</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C19" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="17">
+        <f>2/8</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="17">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="17">
+        <f>1/8</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="17">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="17">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="17">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="17">
+        <f>3/8</f>
+        <v>0.375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Experiment material in English
</commit_message>
<xml_diff>
--- a/experimental-validation/experiment-1-mining-participants/Results.xlsx
+++ b/experimental-validation/experiment-1-mining-participants/Results.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DellPhoto\Documents\Github\IoT-Mining-DSL\experimental-validation\experiment-1-mining-participants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F6C3BD-D734-4B26-A3B8-7E7C92612F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D5943E-7A13-47F8-B5B5-2A3A48C27F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{316D7274-BD52-4D7F-AE2D-2EF32EDE85AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{316D7274-BD52-4D7F-AE2D-2EF32EDE85AF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Encuesta 1" sheetId="3" r:id="rId1"/>
-    <sheet name="Encuesta 2" sheetId="4" r:id="rId2"/>
-    <sheet name="Encuesta 3" sheetId="5" r:id="rId3"/>
-    <sheet name="Errores en los modelos" sheetId="2" r:id="rId4"/>
+    <sheet name="Questionnaire-Q0" sheetId="3" r:id="rId1"/>
+    <sheet name="Questionnaire-Q1" sheetId="4" r:id="rId2"/>
+    <sheet name="Questionnaire-Q2" sheetId="5" r:id="rId3"/>
+    <sheet name="Modeling errors" sheetId="2" r:id="rId4"/>
     <sheet name="Graphs" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -39,47 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="91">
-  <si>
-    <t>Regiones</t>
-  </si>
-  <si>
-    <t>Puntos de control</t>
-  </si>
-  <si>
-    <t>Sensores</t>
-  </si>
-  <si>
-    <t>Actuadores</t>
-  </si>
-  <si>
-    <t>Condicion</t>
-  </si>
-  <si>
-    <t>Adaptacion</t>
-  </si>
-  <si>
-    <t>Regla 1</t>
-  </si>
-  <si>
-    <t>Regla 2</t>
-  </si>
-  <si>
-    <t>Regla 3</t>
-  </si>
-  <si>
-    <t>Errores</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="82">
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Teimpo E1 (min)</t>
-  </si>
-  <si>
-    <t>Tiempo E2 (min)</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
@@ -89,17 +53,95 @@
     <t>Mining knowledge</t>
   </si>
   <si>
-    <t>¿Conoce la terminología utilizada en el diseño de la estructura de una mina de carbón?</t>
-  </si>
-  <si>
-    <t>¿Conoce o ha interactuado alguna vez con sistemas de monitoreo o control en minas subterráneas de carbón?</t>
-  </si>
-  <si>
-    <t>¿Conoce o ha usado alguna herramienta para modelar o representar (ej. gráficamente) una mina subterránea de carbón?</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Regions</t>
+  </si>
+  <si>
+    <t>Control points</t>
+  </si>
+  <si>
+    <t>Sensors</t>
+  </si>
+  <si>
+    <t>Actuators</t>
+  </si>
+  <si>
+    <t>Rule-conditions</t>
+  </si>
+  <si>
+    <t>Rule-actions</t>
+  </si>
+  <si>
+    <t>Mine structure</t>
+  </si>
+  <si>
+    <t>Control points, sensors and actuators</t>
+  </si>
+  <si>
+    <t>Adaptation rules</t>
+  </si>
+  <si>
+    <t>Very easy</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Correctly modeled</t>
+  </si>
+  <si>
+    <t>Incorrectly modeled</t>
+  </si>
+  <si>
+    <t>Time E1 (min)</t>
+  </si>
+  <si>
+    <t>Time E2 (min)</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Rule 1</t>
+  </si>
+  <si>
+    <t>Rule 2</t>
+  </si>
+  <si>
+    <t>Rule 3</t>
+  </si>
+  <si>
+    <t>Errors</t>
+  </si>
+  <si>
+    <t>Adaptation</t>
+  </si>
+  <si>
+    <t>Participant</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Do you understand the terminology used in the design of a coal mine structure?</t>
+  </si>
+  <si>
+    <t>Do you know or have you ever interacted with monitoring or control systems in underground coal mines?</t>
+  </si>
+  <si>
+    <t>Do you know of or have you used any tools to model or represent (e.g. graphically) an underground coal mine?</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Si su respuesta anterior fue </t>
+      <t xml:space="preserve">If your previous answer was </t>
     </r>
     <r>
       <rPr>
@@ -110,7 +152,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Si</t>
+      <t>Yes</t>
     </r>
     <r>
       <rPr>
@@ -120,222 +162,152 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> ¿Cuál(es) de los siguientes aspectos permite representar la herramienta?</t>
+      <t>, which of the following aspects allows you to represent the tool?</t>
     </r>
   </si>
   <si>
-    <t>¿Conoce o ha utilizado el software Meta Programming System (MPS) de Jetbrains?</t>
-  </si>
-  <si>
-    <t>Electrónico</t>
-  </si>
-  <si>
-    <t>Electromecánico</t>
-  </si>
-  <si>
-    <t>Industrial</t>
-  </si>
-  <si>
-    <t>Sistemas</t>
-  </si>
-  <si>
-    <t>Minas</t>
-  </si>
-  <si>
-    <t>Automatización</t>
-  </si>
-  <si>
-    <t>Industria</t>
-  </si>
-  <si>
-    <t>Academia</t>
-  </si>
-  <si>
-    <t>Sector</t>
-  </si>
-  <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Si, Autocad</t>
-  </si>
-  <si>
-    <t>Si, Autocad y Minesight</t>
-  </si>
-  <si>
-    <t>Estructura de la mina</t>
-  </si>
-  <si>
-    <t>Si, Autocad y VentSim</t>
-  </si>
-  <si>
-    <t>Estr. de la mina y sist. de ventilación</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nivel de dificultad para modelar la estructura de la mina </t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Agregaría (o modificaría) algún concepto al lenguaje para representar la estructura de una mina? ¿Cuál? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nivel de dificultad para modelar los puntos de control, los sensores y los actuadores </t>
-  </si>
-  <si>
-    <t>Problemas modelando los puntos de control, los sensores, y los actuadores</t>
-  </si>
-  <si>
-    <t>Problemas modelando la estructura de la mina</t>
-  </si>
-  <si>
-    <t>¿Permite el lenguaje modelar la estructura de las minas subterráneas de carbón que conoce o que ha explorado antes?</t>
-  </si>
-  <si>
-    <t>¿Permite el lenguaje modelar los sensores y actuadores usados para monitoreo y control en min...?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Agregaría (o modificaría) alguna característica del lenguaje para modelar los puntos de control, sensores, y actuadores del sistema? ¿Cuál? </t>
-  </si>
-  <si>
-    <t>Bajo</t>
-  </si>
-  <si>
-    <t>Alto</t>
-  </si>
-  <si>
-    <t>Medio</t>
-  </si>
-  <si>
-    <t>Fácil</t>
-  </si>
-  <si>
-    <t>Muy fácil</t>
-  </si>
-  <si>
-    <t>Intermedio</t>
-  </si>
-  <si>
-    <t>Algunos problemas aprendiendo el uso de la herramienta</t>
-  </si>
-  <si>
-    <t>El modelado para indicar la conexión entre los túneles y cámaras de la mina</t>
-  </si>
-  <si>
-    <t>Es importante que se puede especificar la conexión entre túneles o galerías y su ubicación exacta</t>
-  </si>
-  <si>
-    <t>En los túneles internos relacionar la ubicación dentro de la mina</t>
-  </si>
-  <si>
-    <t>Recomendaría el uso de una especie de GUI que facilite el uso de la herramienta a alguien que no tenga un background en programación</t>
-  </si>
-  <si>
-    <t>Aunque el lenguaje permita representar cualquier parte de la mina usando el elemento “Other”, sería bueno incluir una opción para agregar tambores.  También sería interesante agregar algo para representar también la conexión entre las partes de la mina. Creo que el lenguaje actual mas que permitir modelar la estructura de la mina, permite modelar las regiones.  Finalmente agregaría también los frentes de preparación</t>
-  </si>
-  <si>
-    <t>En la realidad, un solo acceso inclinado podría tener varios puntos de control. Entonces sería interesante modelar la ubicación exacta que tiene un punto de control en un túnel. Esto se puede hacer indicando la abscisa. También, al crear un punto de control y crear sensores por defecto, sería bueno que se creara una nomenclatura automáticamente. Es decir, que se rellenara el camp ID automáticamente siguiendo cierta nomenclatura</t>
-  </si>
-  <si>
-    <t>Nivel de dificultad para modelar las reglas de adaptación del sistema</t>
-  </si>
-  <si>
-    <t>Problemas modelando las reglas de adaptación</t>
-  </si>
-  <si>
-    <t>¿Permite el lenguaje modelar reglas de adaptación (que involucra sensores y actuadores) típicas de los sistemas de monitoreo y control en las minas subterráneas de carbón?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Agregaría (o modificaría) alguna característica del lenguaje para modelar reglas de adaptación del sistema? ¿Cuál? </t>
-  </si>
-  <si>
-    <t>¿Usaría este lenguaje para modelar el sistema IoT y sus reglas de adaptación para una mina subterránea de carbón real?</t>
-  </si>
-  <si>
-    <t>He tenido problemas realizando la regla de adaptación número 3. Al principio no fue fácil agregar nuevas acciones a la lista</t>
-  </si>
-  <si>
-    <t>Creo que es importante incluir reglas de adaptación que involucren la hora del día. Por ejemplo, activar los ventiladores dos horas antes de la jornada laboral es algo que se realiza comúnmente.</t>
-  </si>
-  <si>
-    <t>Si. Es dinámico, de práctica, interesante y su curva de aprendizaje es muy corta.</t>
-  </si>
-  <si>
-    <t>Si. Permite la planeación de sistemas IoT desplegados en las minas de carbón y brinda información necesaria para tratar temas de cobertura de sensado y de comunicación</t>
-  </si>
-  <si>
-    <t>Si. Creo que el lenguaje permite representar completamente el sistema de monitoreo o sistema IoT de las minas subterráneas de carbón, de una forma que no es complicada para usuarios de minería que no son expertos en la configuración de estos sistemas. Este lenguaje, que tienen una curva de aprendizaje favorable, puede favorecer el manejo de los sistemas dentro de una mina.</t>
-  </si>
-  <si>
-    <t>Sugerencias al tooltip de la sintaxis para las reglas de adaptación en los condicionales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si. Luego de un poco de prácticas se puede hacer uso adecuado y facil de la herramienta con resultados interesantes. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si. Permite diseñar los diferentes espacios dentro de la mina junto a puntos de interés como puntos de control, áreas de trabajo y actuadores que permiten una operación segura de la mina. Según el usuario final sería recomendable una interfaz gráfica más amigable.
-</t>
-  </si>
-  <si>
-    <t>Si. Es indiscutible que el profesional que va a estar encargado de modelar la mina y sus elementos debe tener conocimientos tanto de minería como de instrumentación básica y matemática lógica. El sistema inicialmente puede verse complejo, pero con una pequeña inducción o con manuales bien definidos se asimila el manejo rápidamente. Una mejora sustancial puede ser la implementación de una interfaz gráfica, sin embargo la aplicación es completamente funcional y entendible en la interfaz que presenta actualmente</t>
-  </si>
-  <si>
-    <t>Facil</t>
-  </si>
-  <si>
-    <t>Si. La curva de aprendizaje es corta y el software favorece la gestión autonoma de los sistemas de monitoreo dentro de la mina.</t>
-  </si>
-  <si>
-    <t>Si. El software es fácil de utilizar e intuitivo. Sería interesante ver la implementación y operación del sistema IoT dentro de la mina</t>
-  </si>
-  <si>
-    <t>Participante</t>
-  </si>
-  <si>
-    <t>Regions</t>
-  </si>
-  <si>
-    <t>Control points</t>
-  </si>
-  <si>
-    <t>Sensors</t>
-  </si>
-  <si>
-    <t>Actuators</t>
-  </si>
-  <si>
-    <t>Rule-conditions</t>
-  </si>
-  <si>
-    <t>Rule-actions</t>
-  </si>
-  <si>
-    <t>Mine structure</t>
-  </si>
-  <si>
-    <t>Control points, sensors and actuators</t>
-  </si>
-  <si>
-    <t>Adaptation rules</t>
-  </si>
-  <si>
-    <t>Very easy</t>
-  </si>
-  <si>
-    <t>Easy</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Correctly modeled</t>
-  </si>
-  <si>
-    <t>Incorrectly modeled</t>
+    <t>Do you know or have you used Jetbrains Meta Programming System (MPS) software?</t>
+  </si>
+  <si>
+    <t>Mine structure and ventilation system</t>
+  </si>
+  <si>
+    <t>Yes, Autocad</t>
+  </si>
+  <si>
+    <t>Yes, Autocad and VentSim</t>
+  </si>
+  <si>
+    <t>Yes, Autocad and Minesight</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Electronics Eng.</t>
+  </si>
+  <si>
+    <t>Electromechanical Eng.</t>
+  </si>
+  <si>
+    <t>Industrial Eng.</t>
+  </si>
+  <si>
+    <t>Computer Eng.</t>
+  </si>
+  <si>
+    <t>Mining Eng.</t>
+  </si>
+  <si>
+    <t>Automation Eng.</t>
+  </si>
+  <si>
+    <t>Difficulty level for modeling the mine structure</t>
+  </si>
+  <si>
+    <t>Does the language allow you to model the structure of underground coal mines you know or have explored before?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would you add (or modify) any concept to the language to represent the structure of a mine? Which one? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difficulty level for modeling control points, sensors and actuators. </t>
+  </si>
+  <si>
+    <t>Limitations or issues modeling the mine structure</t>
+  </si>
+  <si>
+    <t>Limitation or issues modeling the control points, sensors, and actuators.</t>
+  </si>
+  <si>
+    <t>Does the language allow modeling of sensors and actuators used for monitoring and control in underground coal mining?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would you add (or modify) any language feature to model the control points, sensors, and actuators of the system? Which one? </t>
+  </si>
+  <si>
+    <t>Very Easy</t>
+  </si>
+  <si>
+    <t>Some problems learning how to use the tool</t>
+  </si>
+  <si>
+    <t>I would recommend the use of some sort of GUI to facilitate the use of the tool for someone who does not have a background in programming.</t>
+  </si>
+  <si>
+    <t>In internal tunnels relate the location within the mine.</t>
+  </si>
+  <si>
+    <t>It is important that the connection between tunnels or galleries and their exact location can be specified.</t>
+  </si>
+  <si>
+    <t>Modeling to show the connection between mine tunnels and chambers</t>
+  </si>
+  <si>
+    <t>Although the language allows to represent any part of the mine using the "Other" element, it would be nice to include an option to add drums.  It would also be interesting to add something to represent also the connection between the parts of the mine. I think that the current language more than allowing to model the mine structure, allows to model the regions.  Finally, I would also add the preparation fronts</t>
+  </si>
+  <si>
+    <t>Actually, a single inclined access could have several control points. It would then be interesting to model the exact location that a control point has in a tunnel. This can be done by indicating the abscissa. Also, when creating a control point and creating default sensors, it would be nice to have a nomenclature automatically created. That is to say, to fill in the camp ID automatically following a certain nomenclature.</t>
+  </si>
+  <si>
+    <t>Level of difficulty in modeling system adaptation rules.</t>
+  </si>
+  <si>
+    <t>Limitations or issues modeling adaptation rules</t>
+  </si>
+  <si>
+    <t>Does the language allow modeling of adaptation rules (involving sensors and actuators) typical of monitoring and control systems in underground coal mines?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would you add (or modify) any language feature to model system adaptation rules? Which one? </t>
+  </si>
+  <si>
+    <t>Would you use this language to model the IoT system and its adaptation rules for a real underground coal mine?</t>
+  </si>
+  <si>
+    <t>I have had problems performing adaptation rule number 3. At first it was not easy to add new actions to the list.</t>
+  </si>
+  <si>
+    <t>I think it is important to include adaptation rules that involve the time of day. For example, turning on fans two hours before the workday is commonly done.</t>
+  </si>
+  <si>
+    <t>Suggestions to the syntax tooltip for adaptive rules in conditionals</t>
+  </si>
+  <si>
+    <t>Yes, the learning curve is short and the software favors the autonomous management of the monitoring systems within the mine.</t>
+  </si>
+  <si>
+    <t>Yes, it is dynamic, practical, interesting and its learning curve is very short.</t>
+  </si>
+  <si>
+    <t>Yes. Enables planning of IoT systems deployed in coal mines and provides information needed to address sensing and communication coverage issues.</t>
+  </si>
+  <si>
+    <t>Yes. I believe that the language allows to fully represent the monitoring system or IoT system of subway coal mines, in a way that is not complicated for mining users who are not experts in the configuration of these systems. This language, which have a favorable learning curve, can favor the management of the systems inside a mine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, after a little practice you can make proper and easy use of the tool with interesting results. </t>
+  </si>
+  <si>
+    <t>Yes, it is indisputable that the professional who will be in charge of modeling the mine and its elements must have knowledge of mining as well as basic instrumentation and mathematical logic. The system may initially seem complex, but with a small induction or with well-defined manuals the handling is quickly assimilated. A substantial improvement could be the implementation of a graphical interface, however the application is fully functional and understandable in the current interface.</t>
+  </si>
+  <si>
+    <t>Yes, it allows to design the different spaces inside the mine together with points of interest such as control points, work areas and actuators that allow a safe operation of the mine. Depending on the end user, a more user-friendly graphical interface would be recommended.</t>
+  </si>
+  <si>
+    <t>Yes. The software is easy to use and intuitive. It would be interesting to see the implementation and operation of the IoT system inside the mine.</t>
   </si>
 </sst>
 </file>
@@ -3066,49 +3038,49 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
     <col min="6" max="6" width="25.33203125" customWidth="1"/>
     <col min="7" max="7" width="29.21875" customWidth="1"/>
-    <col min="8" max="8" width="30.5546875" customWidth="1"/>
+    <col min="8" max="8" width="33.77734375" customWidth="1"/>
     <col min="9" max="9" width="24.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -3116,28 +3088,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -3145,28 +3117,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3174,28 +3146,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -3203,28 +3175,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -3232,28 +3204,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -3261,28 +3233,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -3290,28 +3262,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
       </c>
       <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
         <v>35</v>
       </c>
-      <c r="H8" t="s">
-        <v>36</v>
-      </c>
       <c r="I8" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -3319,28 +3291,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3353,13 +3325,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F1774B-7B5A-4EF1-B01F-DCE91DFE08F2}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
     <col min="2" max="2" width="19.109375" customWidth="1"/>
     <col min="3" max="3" width="22.109375" customWidth="1"/>
     <col min="4" max="4" width="31.5546875" customWidth="1"/>
@@ -3372,31 +3344,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -3404,16 +3376,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -3421,19 +3393,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -3441,16 +3413,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -3458,19 +3430,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -3478,42 +3450,42 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
@@ -3521,22 +3493,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -3544,16 +3516,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -3617,8 +3589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8027B0F1-5B6C-4E98-9DEF-D327C416CE08}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3633,22 +3605,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3656,16 +3628,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>74</v>
@@ -3676,79 +3648,79 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="144" x14ac:dyDescent="0.3">
@@ -3756,19 +3728,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3776,19 +3748,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3796,19 +3768,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3822,7 +3794,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3844,16 +3816,16 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E1" s="24"/>
       <c r="F1" s="24"/>
@@ -3870,27 +3842,27 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="25" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="I2" s="24"/>
       <c r="J2" s="24" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="K2" s="24"/>
       <c r="L2" s="24" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="M2" s="24"/>
     </row>
@@ -3903,22 +3875,22 @@
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
       <c r="H3" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -4251,7 +4223,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B12" s="3">
         <f>AVERAGE(B4:B10)</f>
@@ -4358,7 +4330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A455FC-9176-4410-9CB7-E1069F926B92}">
   <dimension ref="B2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
@@ -4372,15 +4344,15 @@
   <sheetData>
     <row r="2" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C2" s="14" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="C3" s="17">
         <v>0.96</v>
@@ -4392,7 +4364,7 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="C4" s="17">
         <v>1</v>
@@ -4403,7 +4375,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>79</v>
+        <v>8</v>
       </c>
       <c r="C5" s="17">
         <f>39/42</f>
@@ -4416,7 +4388,7 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="C6" s="17">
         <f>24/28</f>
@@ -4429,7 +4401,7 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="C7" s="17">
         <v>0.88</v>
@@ -4440,7 +4412,7 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="C8" s="17">
         <v>1</v>
@@ -4451,18 +4423,18 @@
     </row>
     <row r="19" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C19" s="19" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>84</v>
+        <v>13</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="C20" s="17">
         <f>2/8</f>
@@ -4471,7 +4443,7 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="C21" s="17">
         <v>0.62</v>
@@ -4479,7 +4451,7 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="C22" s="17">
         <f>1/8</f>
@@ -4488,7 +4460,7 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="D23" s="17">
         <v>0.13</v>
@@ -4496,7 +4468,7 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="D24" s="17">
         <v>0.87</v>
@@ -4504,7 +4476,7 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="E25" s="17">
         <v>0.62</v>
@@ -4512,7 +4484,7 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="E26" s="17">
         <f>3/8</f>

</xml_diff>